<commit_message>
post class 20 and 21
</commit_message>
<xml_diff>
--- a/docs/wfa-4313-class-roster.xlsx
+++ b/docs/wfa-4313-class-roster.xlsx
@@ -16,6 +16,9 @@
     <sheet name="Grades" sheetId="3" r:id="rId2"/>
     <sheet name="Lab-Roster" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="citation" localSheetId="1">Grades!$Q$3</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="109">
   <si>
     <t>Amacker, Caleb Agustus</t>
   </si>
@@ -281,6 +284,78 @@
   </si>
   <si>
     <t>Quiz 2</t>
+  </si>
+  <si>
+    <t>Brief Submission</t>
+  </si>
+  <si>
+    <t>Late 2 hours</t>
+  </si>
+  <si>
+    <t>Towards a balanced presentation and objective interpretation of acoustic and trawl survey data, with specific reference to the eastern Scotian Shelf</t>
+  </si>
+  <si>
+    <t>The effects of fisheries management practises on freshwater ecosystems</t>
+  </si>
+  <si>
+    <t>Using reverse-time egg transport analysis for predicting Asian carp spawning grounds in the Illinois River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implications of piscine predator control on the federally listed fountain darter. </t>
+  </si>
+  <si>
+    <t>Management issues in the Lake Victoria watershed</t>
+  </si>
+  <si>
+    <t>Growth response of largemouth bass (Micropterus salmoides) to catch-and-release angling: a 27-year mark–recapture study</t>
+  </si>
+  <si>
+    <t>Tracking bowfin with acoustic telemetry: Insight into the ecology of a living fossil</t>
+  </si>
+  <si>
+    <t>Contrasting patterns of productivity and survival rates for stream-type chinook salmon (Oncorhynchus tshawytscha) populations of the Snake and Columbia rivers</t>
+  </si>
+  <si>
+    <t>Relatedness and body size influence territorial behaviour in Salmo salar juveniles in the wild.</t>
+  </si>
+  <si>
+    <t>Red Snapper Distribution on Natural Habitats and Artificial Structures in the Northern Gulf of Mexico</t>
+  </si>
+  <si>
+    <t>Temperature and hydrologic alteration predict the spread of invasive Largemouth Bass (Micropterus salmoides)</t>
+  </si>
+  <si>
+    <t>Predictive Evaluation of Size Restrictions as Management Strategies for Tennessee Reservoir Crappie Fisheries</t>
+  </si>
+  <si>
+    <t>Accounting for variable recruitment and fishing mortality in 1 length-based stock assessments for data-limited fisheries</t>
+  </si>
+  <si>
+    <t>GIS visualisation and analysis of mobile hydroacoustic fisheries data: a practical example</t>
+  </si>
+  <si>
+    <t>Public Perception of Agricultural Pollution and Gulf of Mexico Hypoxia</t>
+  </si>
+  <si>
+    <t>Assessing a social norms approach for improving recreational fisheries compliance</t>
+  </si>
+  <si>
+    <t>Effects of hot dry summers on the loss of Atlantic salmon, Salmo salar, from estuaries in South West England</t>
+  </si>
+  <si>
+    <t>Comparing commercial and recreational harvest characteristics of paddlefish Polyodon spathula (Walbaum, 1792) in the Middle Mississippi River</t>
+  </si>
+  <si>
+    <t>Effects of Multiple Low-Head Dams on Fish, Macroinvertebrates, Habitat, and Water Quality in the Fox River, Illinois</t>
+  </si>
+  <si>
+    <t>Effectively managing angler satisfaction in recreational fisheries requires understanding the fish species and the anglers</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>Influence of behavior and mating success on brood-specific contribution to fish recruitment in ponds</t>
   </si>
 </sst>
 </file>
@@ -1838,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1850,7 +1925,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -1893,8 +1968,11 @@
       <c r="O1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1904,8 +1982,14 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1915,8 +1999,14 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1926,8 +2016,14 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1937,8 +2033,11 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1948,8 +2047,14 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1959,8 +2064,14 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1970,8 +2081,14 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1981,8 +2098,14 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1992,8 +2115,14 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2003,8 +2132,14 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2014,8 +2149,14 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2025,8 +2166,14 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2036,8 +2183,14 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2047,8 +2200,14 @@
       <c r="C15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2058,8 +2217,14 @@
       <c r="C16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2070,7 +2235,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2080,8 +2245,14 @@
       <c r="C18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2091,8 +2262,11 @@
       <c r="C19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2102,8 +2276,14 @@
       <c r="C20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2113,8 +2293,14 @@
       <c r="C21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2124,8 +2310,14 @@
       <c r="C22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2135,8 +2327,14 @@
       <c r="C23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2146,8 +2344,14 @@
       <c r="C24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -2157,8 +2361,14 @@
       <c r="C25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -2171,6 +2381,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="599" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2179,13 +2390,15 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>